<commit_message>
Actualización automática 2025-05-22 10:10:05
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1589,7 +1589,7 @@
         <v>11287.86</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>374.67</v>
       </c>
     </row>
     <row r="7">
@@ -1891,7 +1891,7 @@
         <v>25470.65</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>12134.62</v>
+        <v>12509.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-22 10:15:06
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1589,7 +1589,7 @@
         <v>11287.86</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>374.67</v>
+        <v>2867.6</v>
       </c>
     </row>
     <row r="7">
@@ -1891,7 +1891,7 @@
         <v>25470.65</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>12509.29</v>
+        <v>15002.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-27 14:55:07
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0</v>
+        <v>-49.25</v>
       </c>
     </row>
     <row r="3">
@@ -1891,7 +1891,7 @@
         <v>25470.65</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>17787.32</v>
+        <v>17738.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-27 15:20:07
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0</v>
+        <v>40.19</v>
       </c>
     </row>
     <row r="15">
@@ -1891,7 +1891,7 @@
         <v>25470.65</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>17738.07</v>
+        <v>17778.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-29 15:55:07
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1877,7 +1877,7 @@
         <v>7441.92</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>8696.879999999999</v>
+        <v>8859.700000000001</v>
       </c>
     </row>
     <row r="19">
@@ -1891,7 +1891,7 @@
         <v>25470.65</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>17778.26</v>
+        <v>17941.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-30 12:30:07
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1437,7 +1437,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1877,7 +1877,7 @@
         <v>7441.92</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>8859.700000000001</v>
+        <v>24096.93</v>
       </c>
     </row>
     <row r="19">
@@ -1891,7 +1891,7 @@
         <v>25470.65</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>17941.08</v>
+        <v>33178.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-04 15:35:07
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0</v>
+        <v>-22.68</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>0</v>
@@ -1437,7 +1437,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -1661,7 +1661,7 @@
         <v>2785.1</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0</v>
+        <v>-22.68</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>0</v>
@@ -1948,7 +1948,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>0</v>
+        <v>-22.68</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-06-09 10:05:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>1267.19</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>0</v>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>0 de 17</t>
+          <t>1 de 17</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
@@ -1441,7 +1441,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -1854,7 +1854,7 @@
         <v>4277.03</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0</v>
+        <v>1267.19</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>0</v>
@@ -1952,7 +1952,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>95.25999999999999</v>
+        <v>1362.45</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -1980,8 +1980,8 @@
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2056,13 +2056,13 @@
         <v>8668.91</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>1267.19</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>8668.91</v>
+        <v>7401.719999999999</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.1461763935719716</v>
       </c>
     </row>
     <row r="4">
@@ -2435,13 +2435,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>95.26000000000001</v>
+        <v>1362.45</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>47124.04386304603</v>
+        <v>45856.85386304604</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.002017395264366673</v>
+        <v>0.02885366552526111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-16 15:20:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>117.94</v>
+        <v>15693.84</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>0</v>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>0</v>
+        <v>4481.57</v>
       </c>
       <c r="N18" s="2" t="n">
         <v>0</v>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="M19" s="4" t="inlineStr">
         <is>
-          <t>1 de 17</t>
+          <t>2 de 17</t>
         </is>
       </c>
       <c r="N19" s="4" t="inlineStr">
@@ -1689,7 +1689,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -1859,7 +1859,7 @@
         <v>2867.6</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>117.94</v>
+        <v>15693.84</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
@@ -2183,7 +2183,7 @@
         <v>24096.93</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>4481.57</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>1362.45</v>
+        <v>21419.92</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -2228,9 +2228,9 @@
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2616,13 +2616,13 @@
         <v>28209.84</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>95.26000000000001</v>
+        <v>20152.73</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>28114.58</v>
+        <v>8057.110000000001</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.003376835884216288</v>
+        <v>0.7143865402994133</v>
       </c>
     </row>
     <row r="17">
@@ -2683,13 +2683,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1362.45</v>
+        <v>21419.92</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>45856.85386304604</v>
+        <v>25799.38386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.02885366552526111</v>
+        <v>0.4536263402384314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-17 14:20:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>0</v>
+        <v>-18.25</v>
       </c>
       <c r="N15" s="2" t="n">
         <v>0</v>
@@ -2102,7 +2102,7 @@
         <v>4277.03</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>1267.19</v>
+        <v>1248.94</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>21419.92</v>
+        <v>21401.67</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -2616,13 +2616,13 @@
         <v>28209.84</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>20152.73</v>
+        <v>20134.48</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>8057.110000000001</v>
+        <v>8075.360000000001</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.7143865402994133</v>
+        <v>0.7137396029186979</v>
       </c>
     </row>
     <row r="17">
@@ -2683,13 +2683,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>21419.92</v>
+        <v>21401.67</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>25799.38386304603</v>
+        <v>25817.63386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4536263402384314</v>
+        <v>0.4532398457646261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 11:40:10
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0</v>
+        <v>748.52</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>0</v>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="H19" s="4" t="inlineStr">
         <is>
-          <t>0 de 17</t>
+          <t>1 de 17</t>
         </is>
       </c>
       <c r="I19" s="4" t="inlineStr">
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0</v>
+        <v>748.52</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>21401.67</v>
+        <v>22150.19</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -2400,13 +2400,13 @@
         <v>800</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>748.52</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>800</v>
+        <v>51.48000000000002</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>0.93565</v>
       </c>
     </row>
     <row r="8">
@@ -2683,13 +2683,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>21401.67</v>
+        <v>22150.19</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>25817.63386304603</v>
+        <v>25069.11386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4532398457646261</v>
+        <v>0.4690918371910773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 13:55:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -713,7 +713,7 @@
         <v>748.52</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0</v>
+        <v>129.36</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="I19" s="4" t="inlineStr">
         <is>
-          <t>0 de 17</t>
+          <t>1 de 17</t>
         </is>
       </c>
       <c r="J19" s="4" t="inlineStr">
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>748.52</v>
+        <v>877.88</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>22150.19</v>
+        <v>22279.55</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -2424,13 +2424,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>129.36</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>625</v>
+        <v>495.64</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0</v>
+        <v>0.206976</v>
       </c>
     </row>
     <row r="9">
@@ -2683,13 +2683,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>22150.19</v>
+        <v>22279.55</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>25069.11386304603</v>
+        <v>24939.75386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4690918371910773</v>
+        <v>0.4718313947325267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-26 14:31:13
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -713,7 +713,7 @@
         <v>748.52</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>129.36</v>
+        <v>29.29</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>877.88</v>
+        <v>777.8099999999999</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>22279.55</v>
+        <v>22179.48</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -2424,13 +2424,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>129.36</v>
+        <v>29.29</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>495.64</v>
+        <v>595.71</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0.206976</v>
+        <v>0.046864</v>
       </c>
     </row>
     <row r="9">
@@ -2683,13 +2683,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>22279.55</v>
+        <v>22179.48</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>24939.75386304603</v>
+        <v>25039.82386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4718313947325267</v>
+        <v>0.4697121343493106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-30 14:35:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>1317.8</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>11.52</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -1361,13 +1361,13 @@
         <v>1267.19</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>0</v>
+        <v>40.74</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>0</v>
@@ -1596,47 +1596,47 @@
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
+          <t>1 de 17</t>
+        </is>
+      </c>
+      <c r="F19" s="4" t="inlineStr">
+        <is>
           <t>0 de 17</t>
         </is>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>1 de 17</t>
+        </is>
+      </c>
+      <c r="H19" s="4" t="inlineStr">
+        <is>
+          <t>1 de 17</t>
+        </is>
+      </c>
+      <c r="I19" s="4" t="inlineStr">
+        <is>
+          <t>1 de 17</t>
+        </is>
+      </c>
+      <c r="J19" s="4" t="inlineStr">
         <is>
           <t>0 de 17</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr">
+      <c r="K19" s="4" t="inlineStr">
         <is>
           <t>0 de 17</t>
         </is>
       </c>
-      <c r="H19" s="4" t="inlineStr">
-        <is>
-          <t>1 de 17</t>
-        </is>
-      </c>
-      <c r="I19" s="4" t="inlineStr">
-        <is>
-          <t>1 de 17</t>
-        </is>
-      </c>
-      <c r="J19" s="4" t="inlineStr">
+      <c r="L19" s="4" t="inlineStr">
         <is>
           <t>0 de 17</t>
         </is>
       </c>
-      <c r="K19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="L19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
       <c r="M19" s="4" t="inlineStr">
         <is>
-          <t>2 de 17</t>
+          <t>4 de 17</t>
         </is>
       </c>
       <c r="N19" s="4" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>3054.27</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>1317.8</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -1967,7 +1967,7 @@
         <v>156.67</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>11.52</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -2102,7 +2102,7 @@
         <v>4277.03</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>2100.7</v>
+        <v>2206.26</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>32556.53</v>
+        <v>33991.41</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -2328,13 +2328,13 @@
         <v>372.993863046034</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>372.993863046034</v>
+        <v>308.173863046034</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>0.1737830201029341</v>
       </c>
     </row>
     <row r="5">
@@ -2376,13 +2376,13 @@
         <v>106.82</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>40.74</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>106.82</v>
+        <v>66.07999999999998</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>0.381389252948886</v>
       </c>
     </row>
     <row r="7">
@@ -2616,13 +2616,13 @@
         <v>28209.84</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>29659.77</v>
+        <v>30989.09</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-1449.93</v>
+        <v>-2779.25</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>1.05139802281757</v>
+        <v>1.098520587142642</v>
       </c>
     </row>
     <row r="17">
@@ -2683,13 +2683,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>32556.53</v>
+        <v>33991.41</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>14662.77386304603</v>
+        <v>13227.89386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.6894750099329362</v>
+        <v>0.7198625820191682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-30 14:40:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>25219.13</v>
+        <v>25364.28</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>0</v>
@@ -1541,13 +1541,13 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0</v>
+        <v>194.46</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>0</v>
+        <v>122.22</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>0</v>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>1 de 17</t>
+          <t>2 de 17</t>
         </is>
       </c>
       <c r="F19" s="4" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>1 de 17</t>
+          <t>2 de 17</t>
         </is>
       </c>
       <c r="H19" s="4" t="inlineStr">
@@ -1859,7 +1859,7 @@
         <v>2867.6</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>25219.13</v>
+        <v>25364.28</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
@@ -2183,7 +2183,7 @@
         <v>24096.93</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>4481.57</v>
+        <v>4798.25</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>37455.34</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>33991.41</v>
+        <v>34453.24</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>0</v>
@@ -2229,7 +2229,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2328,13 +2328,13 @@
         <v>372.993863046034</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>64.81999999999999</v>
+        <v>259.28</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>308.173863046034</v>
+        <v>113.713863046034</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0.1737830201029341</v>
+        <v>0.6951320804117366</v>
       </c>
     </row>
     <row r="5">
@@ -2376,13 +2376,13 @@
         <v>106.82</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>40.74</v>
+        <v>162.96</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>66.07999999999998</v>
+        <v>-56.14000000000001</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.381389252948886</v>
+        <v>1.525557011795544</v>
       </c>
     </row>
     <row r="7">
@@ -2616,13 +2616,13 @@
         <v>28209.84</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>30989.09</v>
+        <v>31134.24</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-2779.25</v>
+        <v>-2924.400000000001</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>1.098520587142642</v>
+        <v>1.103665954858305</v>
       </c>
     </row>
     <row r="17">
@@ -2683,13 +2683,13 @@
         <v>47219.30386304604</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>33991.41</v>
+        <v>34453.24000000001</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>13227.89386304603</v>
+        <v>12766.06386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.7198625820191682</v>
+        <v>0.7296431158732777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-07 14:30:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -931,7 +931,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CONZA VEGA FRANCO BLADYMIR</t>
+          <t>CONSTANTE CAMACHO ARIANA ELIZABETH</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -991,7 +991,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DDH S.A.S.</t>
+          <t>CONZA VEGA FRANCO BLADYMIR</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>F.V - AREA ANDINA S.A.</t>
+          <t>CULMA OVIEDO NINI JOHANA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>6266.88</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FERRIACABADOS MACONSE</t>
+          <t>DDH S.A.S.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
+          <t>F.V - AREA ANDINA S.A.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0</v>
+        <v>6266.88</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MUNDO-CERAMICO CIA.LTDA.</t>
+          <t>FERRIACABADOS MACONSE</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
+          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
+          <t>LUNA PAZMIÑO MYRIAM DEL ROCIO</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
+          <t>MERIZALDE PEREIRA KAREN ELIZABETH</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
+          <t>MUNDIACABADOS CIA. LTDA.</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1531,137 +1531,437 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>MUNDO-CERAMICO CIA.LTDA.</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>ZAMBRANO ANGELA MARIA</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="F19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="G19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="H19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="I19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="J19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="K19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="L19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="M19" s="4" t="inlineStr">
-        <is>
-          <t>1 de 17</t>
-        </is>
-      </c>
-      <c r="N19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="O19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="P19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="Q19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="R19" s="4" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
+      <c r="C23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="L24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="M24" s="4" t="inlineStr">
+        <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="N24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="O24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="P24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="Q24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="R24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
         </is>
       </c>
     </row>
@@ -1676,7 +1976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1900,23 +2200,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CONZA VEGA FRANCO BLADYMIR</t>
+          <t>CONSTANTE CAMACHO ARIANA ELIZABETH</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1183.91</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>2785.1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-22.68</v>
+        <v>2261.64</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1927,23 +2227,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DDH S.A.S.</t>
+          <t>CONZA VEGA FRANCO BLADYMIR</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0</v>
+        <v>1183.91</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0</v>
+        <v>2785.1</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0</v>
+        <v>-22.68</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>1425</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10">
@@ -1954,23 +2254,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>F.V - AREA ANDINA S.A.</t>
+          <t>CULMA OVIEDO NINI JOHANA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>5556.96</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>156.67</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>11.52</v>
+        <v>851.4299999999999</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>6266.88</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>12000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1981,7 +2281,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FERRIACABADOS MACONSE</t>
+          <t>DDH S.A.S.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1997,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>3000</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="12">
@@ -2008,23 +2308,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
+          <t>F.V - AREA ANDINA S.A.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0</v>
+        <v>5556.96</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0</v>
+        <v>156.67</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0</v>
+        <v>11.52</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0</v>
+        <v>6266.88</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>250</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="13">
@@ -2035,7 +2335,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MUNDO-CERAMICO CIA.LTDA.</t>
+          <t>FERRIACABADOS MACONSE</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -2051,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="14">
@@ -2062,14 +2362,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
+          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>40.19</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>0</v>
@@ -2078,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>1500</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15">
@@ -2089,23 +2389,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
+          <t>LUNA PAZMIÑO MYRIAM DEL ROCIO</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>4277.03</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>4321.33</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2116,7 +2416,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
+          <t>MERIZALDE PEREIRA KAREN ELIZABETH</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -2143,11 +2443,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
+          <t>MUNDIACABADOS CIA. LTDA.</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>-545.1799999999999</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>0</v>
@@ -2159,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2170,39 +2470,174 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>MUNDO-CERAMICO CIA.LTDA.</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>40.19</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>4277.03</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>4321.33</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>ZAMBRANO ANGELA MARIA</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C23" s="2" t="n">
         <v>7441.92</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D23" s="2" t="n">
         <v>24096.93</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E23" s="2" t="n">
         <v>4798.25</v>
       </c>
-      <c r="F18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="n">
+      <c r="F23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="n">
         <v>20000</v>
       </c>
     </row>
-    <row r="19">
-      <c r="C19" s="6" t="n">
-        <v>25470.65</v>
-      </c>
-      <c r="D19" s="6" t="n">
+    <row r="24">
+      <c r="C24" s="6" t="n">
+        <v>24925.47</v>
+      </c>
+      <c r="D24" s="6" t="n">
         <v>37455.34</v>
       </c>
-      <c r="E19" s="6" t="n">
-        <v>36568.31</v>
-      </c>
-      <c r="F19" s="6" t="n">
+      <c r="E24" s="6" t="n">
+        <v>39681.38</v>
+      </c>
+      <c r="F24" s="6" t="n">
         <v>6266.88</v>
       </c>
-      <c r="G19" s="6" t="n">
+      <c r="G24" s="6" t="n">
         <v>60225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-16 10:50:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>3317.32</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>1 de 22</t>
+          <t>2 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -2078,7 +2078,7 @@
         <v>1317.8</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>3317.32</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>3500</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>6266.88</v>
+        <v>9584.200000000001</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2663,7 +2663,7 @@
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>6266.88</v>
+        <v>9584.200000000001</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>32489.66</v>
+        <v>29172.34</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1616986449254758</v>
+        <v>0.2472924569633925</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>6266.88</v>
+        <v>9584.200000000001</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51956.12386304603</v>
+        <v>48638.80386304604</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1076358068838418</v>
+        <v>0.1646119122013054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-16 10:55:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>7529.26</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>2 de 22</t>
+          <t>3 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -2348,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>7529.26</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>3000</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>9584.200000000001</v>
+        <v>17113.46</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2663,7 +2663,7 @@
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>9584.200000000001</v>
+        <v>17113.46</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>29172.34</v>
+        <v>21643.08</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2472924569633925</v>
+        <v>0.4415631529543143</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>9584.200000000001</v>
+        <v>17113.46</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>48638.80386304604</v>
+        <v>41109.54386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1646119122013054</v>
+        <v>0.2939295272407245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 10:10:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>6266.88</v>
+        <v>12246.22</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1989,7 +1989,7 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2321,7 +2321,7 @@
         <v>11.52</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>6266.88</v>
+        <v>12246.22</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>12000</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>17480.29</v>
+        <v>23459.63</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2665,7 +2665,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>17480.29</v>
+        <v>23459.63</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>21276.25</v>
+        <v>15296.91</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.451028136154569</v>
+        <v>0.6053076461417867</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>17480.29</v>
+        <v>23459.63</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>40742.71386304603</v>
+        <v>34763.37386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.3002299579238076</v>
+        <v>0.4029271669868232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 14:45:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0</v>
+        <v>132.3</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>0</v>
@@ -965,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0</v>
+        <v>651.72</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>0</v>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>1465.34</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0</v>
+        <v>1372.56</v>
       </c>
       <c r="M10" s="2" t="n">
         <v>0</v>
@@ -1891,52 +1891,52 @@
       </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr">
+      <c r="F24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
+      <c r="G24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="G24" s="4" t="inlineStr">
+      <c r="H24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="H24" s="4" t="inlineStr">
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="I24" s="4" t="inlineStr">
+      <c r="K24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
-      <c r="K24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
       <c r="L24" s="4" t="inlineStr">
         <is>
-          <t>0 de 22</t>
+          <t>1 de 22</t>
         </is>
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>4 de 22</t>
+          <t>5 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -2213,7 +2213,7 @@
         <v>2261.64</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0</v>
+        <v>784.02</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>0</v>
@@ -2267,7 +2267,7 @@
         <v>851.4299999999999</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>2837.9</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>23459.63</v>
+        <v>27081.55</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2739,13 +2739,13 @@
         <v>8668.91</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>1465.34</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>8668.91</v>
+        <v>7203.57</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.1690339385228362</v>
       </c>
     </row>
     <row r="4">
@@ -2859,13 +2859,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>132.3</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>625</v>
+        <v>492.7</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0</v>
+        <v>0.21168</v>
       </c>
     </row>
     <row r="9">
@@ -3027,13 +3027,13 @@
         <v>2501.01</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>1372.56</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>2501.01</v>
+        <v>1128.45</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>0.5488022838773134</v>
       </c>
     </row>
     <row r="16">
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>23459.63</v>
+        <v>24111.35</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>15296.91</v>
+        <v>14645.19</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.6053076461417867</v>
+        <v>0.6221233887235548</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>23459.63</v>
+        <v>27081.55</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>34763.37386304603</v>
+        <v>31141.45386304604</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4029271669868232</v>
+        <v>0.4651348814585738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 17:25:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>5.94</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>5 de 22</t>
+          <t>6 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>5.94</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1425</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>30721.26</v>
+        <v>30727.2</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>27184.28</v>
+        <v>27190.22</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>11572.26</v>
+        <v>11566.32</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.7014114263037928</v>
+        <v>0.7015646907592886</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>30721.26</v>
+        <v>30727.2</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>27501.74386304603</v>
+        <v>27495.80386304604</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5276481452633998</v>
+        <v>0.5277501667945109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-29 11:20:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0</v>
+        <v>5.76</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>0</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>6 de 22</t>
+          <t>7 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -2159,7 +2159,7 @@
         <v>25364.28</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>5.76</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>12000</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>30727.2</v>
+        <v>30732.96</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>27190.22</v>
+        <v>27195.98</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>11566.32</v>
+        <v>11560.56</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.7015646907592886</v>
+        <v>0.7017133108373451</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>30727.2</v>
+        <v>30732.96</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>27495.80386304604</v>
+        <v>27490.04386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5277501667945109</v>
+        <v>0.5278490967640733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-29 11:25:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>5.76</v>
+        <v>2654.94</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>0</v>
@@ -2159,7 +2159,7 @@
         <v>25364.28</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>5.76</v>
+        <v>2654.94</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>12000</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>30732.96</v>
+        <v>33382.14</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2664,7 +2664,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>27195.98</v>
+        <v>29845.16</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>11560.56</v>
+        <v>8911.380000000001</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.7017133108373451</v>
+        <v>0.7700677098626451</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>30732.96</v>
+        <v>33382.14</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>27490.04386304603</v>
+        <v>24840.86386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5278490967640733</v>
+        <v>0.5733496691191425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-29 13:45:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1625,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0</v>
+        <v>33.7</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>0</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>7 de 22</t>
+          <t>8 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>33.7</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>1500</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>33382.14</v>
+        <v>33415.84</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2664,7 +2664,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>29845.16</v>
+        <v>29878.86</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>8911.380000000001</v>
+        <v>8877.68</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.7700677098626451</v>
+        <v>0.7709372405276632</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>33382.14</v>
+        <v>33415.84</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>24840.86386304603</v>
+        <v>24807.16386304604</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5733496691191425</v>
+        <v>0.5739284781424501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-31 15:40:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -641,13 +641,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0</v>
+        <v>445.7</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0</v>
+        <v>127.56</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>0</v>
@@ -1115,13 +1115,13 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0</v>
+        <v>518.4</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0</v>
+        <v>207.38</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
@@ -1133,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0</v>
+        <v>366.3</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>0</v>
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="2" t="n">
-        <v>0</v>
+        <v>130.5</v>
       </c>
     </row>
     <row r="12">
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>0</v>
+        <v>15441.74</v>
       </c>
       <c r="N23" s="2" t="n">
         <v>0</v>
@@ -1886,82 +1886,82 @@
     <row r="24">
       <c r="C24" s="4" t="inlineStr">
         <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="inlineStr">
+        <is>
+          <t>2 de 22</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>2 de 22</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="D24" s="4" t="inlineStr">
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="I24" s="4" t="inlineStr">
         <is>
           <t>2 de 22</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr">
+      <c r="J24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
+      <c r="K24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="G24" s="4" t="inlineStr">
+      <c r="L24" s="4" t="inlineStr">
+        <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="M24" s="4" t="inlineStr">
+        <is>
+          <t>9 de 22</t>
+        </is>
+      </c>
+      <c r="N24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="H24" s="4" t="inlineStr">
+      <c r="O24" s="4" t="inlineStr">
         <is>
           <t>0 de 22</t>
         </is>
       </c>
-      <c r="I24" s="4" t="inlineStr">
+      <c r="P24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="Q24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="R24" s="4" t="inlineStr">
         <is>
           <t>1 de 22</t>
-        </is>
-      </c>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
-      <c r="K24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
-      <c r="L24" s="4" t="inlineStr">
-        <is>
-          <t>1 de 22</t>
-        </is>
-      </c>
-      <c r="M24" s="4" t="inlineStr">
-        <is>
-          <t>8 de 22</t>
-        </is>
-      </c>
-      <c r="N24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
-      <c r="O24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
-      <c r="P24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
-      <c r="Q24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
-        </is>
-      </c>
-      <c r="R24" s="4" t="inlineStr">
-        <is>
-          <t>0 de 22</t>
         </is>
       </c>
     </row>
@@ -2078,7 +2078,7 @@
         <v>1317.8</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>3317.32</v>
+        <v>3890.58</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>3500</v>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>5.94</v>
+        <v>1228.52</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1425</v>
@@ -2618,7 +2618,7 @@
         <v>4798.25</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0</v>
+        <v>15441.74</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>20000</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>33415.84</v>
+        <v>50653.42</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2663,8 +2663,8 @@
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2715,13 +2715,13 @@
         <v>1041.16</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>518.4</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1041.16</v>
+        <v>522.7600000000001</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0</v>
+        <v>0.497906181566714</v>
       </c>
     </row>
     <row r="3">
@@ -2763,13 +2763,13 @@
         <v>372.993863046034</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>653.08</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>372.993863046034</v>
+        <v>-280.086136953966</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>1.750913526208335</v>
       </c>
     </row>
     <row r="5">
@@ -2811,13 +2811,13 @@
         <v>106.82</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>127.56</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>106.82</v>
+        <v>-20.74000000000001</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>1.194158397303876</v>
       </c>
     </row>
     <row r="7">
@@ -2859,13 +2859,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>132.3</v>
+        <v>498.6</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>492.7</v>
+        <v>126.4</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0.21168</v>
+        <v>0.79776</v>
       </c>
     </row>
     <row r="9">
@@ -2979,13 +2979,13 @@
         <v>130</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0</v>
+        <v>130.5</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>130</v>
+        <v>-0.5</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>0</v>
+        <v>1.003846153846154</v>
       </c>
     </row>
     <row r="14">
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>29878.86</v>
+        <v>45320.6</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>8877.68</v>
+        <v>-6564.059999999998</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.7709372405276632</v>
+        <v>1.169366512077703</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>33415.84</v>
+        <v>50653.42</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>24807.16386304604</v>
+        <v>7569.583863046037</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5739284781424501</v>
+        <v>0.8699898088245078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-31 17:10:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>5.94</v>
+        <v>3864.56</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1228.52</v>
+        <v>5087.14</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1425</v>
@@ -2635,7 +2635,7 @@
         <v>39681.38</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>50653.42</v>
+        <v>54512.04</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>60225</v>
@@ -2663,7 +2663,7 @@
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
@@ -3051,13 +3051,13 @@
         <v>38756.54</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45320.6</v>
+        <v>49179.22</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-6564.059999999998</v>
+        <v>-10422.68</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>1.169366512077703</v>
+        <v>1.268926999159368</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>58223.00386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>50653.42</v>
+        <v>54512.04</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>7569.583863046037</v>
+        <v>3710.963863046034</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.8699898088245078</v>
+        <v>0.9362629267329615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-07 16:50:08
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0</v>
+        <v>1090.97</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>0 de 22</t>
+          <t>1 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -1989,7 +1989,7 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2321,7 +2321,7 @@
         <v>12246.22</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0</v>
+        <v>1090.97</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>6000</v>
@@ -2635,7 +2635,7 @@
         <v>60037.18</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>0</v>
+        <v>1090.97</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>48450</v>
@@ -2663,9 +2663,9 @@
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3051,13 +3051,13 @@
         <v>36056.7</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0</v>
+        <v>1090.97</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>36056.7</v>
+        <v>34965.73</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0</v>
+        <v>0.0302570673411599</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>55023.16386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>1090.97</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>55023.16386304603</v>
+        <v>53932.19386304604</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0</v>
+        <v>0.0198274676228261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-08 15:45:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1625,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0</v>
+        <v>-33.7</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>0</v>
@@ -2510,7 +2510,7 @@
         <v>33.7</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>-33.7</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>1000</v>
@@ -2635,7 +2635,7 @@
         <v>60037.18</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>1090.97</v>
+        <v>1057.27</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>48450</v>
@@ -2665,7 +2665,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3051,13 +3051,13 @@
         <v>36056.7</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>1090.97</v>
+        <v>1057.27</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>34965.73</v>
+        <v>34999.43</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.0302570673411599</v>
+        <v>0.02932242828655978</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>55023.16386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1090.97</v>
+        <v>1057.27</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>53932.19386304604</v>
+        <v>53965.89386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.0198274676228261</v>
+        <v>0.01921499829838157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-19 12:15:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0</v>
+        <v>1980.66</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M24" s="4" t="inlineStr">
         <is>
-          <t>1 de 22</t>
+          <t>2 de 22</t>
         </is>
       </c>
       <c r="N24" s="4" t="inlineStr">
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0</v>
+        <v>1980.66</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>2000</v>
@@ -2635,7 +2635,7 @@
         <v>60037.18</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>1057.27</v>
+        <v>3037.93</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>48450</v>
@@ -2665,7 +2665,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3051,13 +3051,13 @@
         <v>36056.7</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>1057.27</v>
+        <v>3037.93</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>34999.43</v>
+        <v>33018.77</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.02932242828655978</v>
+        <v>0.0842542440101285</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>55023.16386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1057.27</v>
+        <v>3037.93</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>53965.89386304603</v>
+        <v>51985.23386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.01921499829838157</v>
+        <v>0.05521183782818233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-19 13:10:10
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>1980.66</v>
+        <v>2161.81</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>1980.66</v>
+        <v>2161.81</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>2000</v>
@@ -2635,7 +2635,7 @@
         <v>60037.18</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>3037.93</v>
+        <v>3219.08</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>48450</v>
@@ -2665,7 +2665,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3051,13 +3051,13 @@
         <v>36056.7</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>3037.93</v>
+        <v>3219.08</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>33018.77</v>
+        <v>32837.62</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.0842542440101285</v>
+        <v>0.08927827560481132</v>
       </c>
     </row>
     <row r="17">
@@ -3118,13 +3118,13 @@
         <v>55023.16386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3037.93</v>
+        <v>3219.08</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51985.23386304603</v>
+        <v>51804.08386304603</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.05521183782818233</v>
+        <v>0.05850408762412076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-19 15:45:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0</v>
+        <v>-81.41</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0</v>
@@ -2618,7 +2618,7 @@
         <v>16408.39</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0</v>
+        <v>-81.41</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>20000</v>
@@ -2635,7 +2635,7 @@
         <v>60037.18</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>3219.08</v>
+        <v>3137.67</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>48450</v>
@@ -2665,7 +2665,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2739,13 +2739,13 @@
         <v>8668.91</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>-81.41</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>8668.91</v>
+        <v>8750.32</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>-0.009391030706282565</v>
       </c>
     </row>
     <row r="4">
@@ -3118,13 +3118,13 @@
         <v>55023.16386304603</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3219.08</v>
+        <v>3137.67</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51804.08386304603</v>
+        <v>51885.49386304604</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.05850408762412076</v>
+        <v>0.05702452893857096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 12:40:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1925,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>0</v>
+        <v>9735.9</v>
       </c>
       <c r="N24" s="2" t="n">
         <v>0</v>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="M25" s="4" t="inlineStr">
         <is>
-          <t>3 de 23</t>
+          <t>4 de 23</t>
         </is>
       </c>
       <c r="N25" s="4" t="inlineStr">
@@ -2705,7 +2705,7 @@
         <v>-81.41</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>0</v>
+        <v>9735.9</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>20000</v>
@@ -2722,7 +2722,7 @@
         <v>8424.639999999999</v>
       </c>
       <c r="F25" s="6" t="n">
-        <v>20470.79</v>
+        <v>30206.69</v>
       </c>
       <c r="G25" s="6" t="n">
         <v>48450</v>
@@ -3042,13 +3042,13 @@
         <v>43100.0854117774</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>19657.67</v>
+        <v>29393.57</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>23442.4154117774</v>
+        <v>13706.5154117774</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.4560935277086111</v>
+        <v>0.6819840313348429</v>
       </c>
     </row>
     <row r="13">
@@ -3109,13 +3109,13 @@
         <v>58203.46623249458</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>20470.79</v>
+        <v>30206.69</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>37732.67623249458</v>
+        <v>27996.77623249458</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.3517108400078637</v>
+        <v>0.5189843828087307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-29 08:55:10
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1745,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>1244.13</v>
+        <v>1632.93</v>
       </c>
       <c r="N21" s="2" t="n">
         <v>0</v>
@@ -2684,7 +2684,7 @@
         <v>-33.7</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>1244.13</v>
+        <v>1632.93</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>1000</v>
@@ -2809,7 +2809,7 @@
         <v>8424.639999999999</v>
       </c>
       <c r="F26" s="6" t="n">
-        <v>20529.03</v>
+        <v>20917.83</v>
       </c>
       <c r="G26" s="6" t="n">
         <v>48450</v>
@@ -3129,13 +3129,13 @@
         <v>43100.0854117774</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>20277.11</v>
+        <v>20665.91</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>22822.9754117774</v>
+        <v>22434.1754117774</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.4704656569998151</v>
+        <v>0.4794865207935968</v>
       </c>
     </row>
     <row r="13">
@@ -3196,13 +3196,13 @@
         <v>58203.46623249458</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>20529.03</v>
+        <v>20917.83</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>37674.43623249458</v>
+        <v>37285.63623249458</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.3527114676984442</v>
+        <v>0.3593914822262205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-13 17:30:09
</commit_message>
<xml_diff>
--- a/data/RIOS CARRION ANGEL BENIGNO.xlsx
+++ b/data/RIOS CARRION ANGEL BENIGNO.xlsx
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>195.64</v>
+        <v>5872.12</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -2711,7 +2711,7 @@
         <v>-347.92</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>195.64</v>
+        <v>5872.12</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>2000</v>
@@ -2809,7 +2809,7 @@
         <v>23879.02</v>
       </c>
       <c r="F26" s="6" t="n">
-        <v>9672.959999999999</v>
+        <v>15349.44</v>
       </c>
       <c r="G26" s="6" t="n">
         <v>48450</v>
@@ -3129,13 +3129,13 @@
         <v>27954.98</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>11064.99</v>
+        <v>16741.47</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>16889.99</v>
+        <v>11213.51</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.3958146276620481</v>
+        <v>0.5988725443552455</v>
       </c>
     </row>
     <row r="13">
@@ -3172,13 +3172,13 @@
         <v>42203.38110009469</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>9672.959999999999</v>
+        <v>15349.44</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>32530.42110009469</v>
+        <v>26853.94110009469</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.2291986980156502</v>
+        <v>0.3637016655986731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>